<commit_message>
Updated User stories and sprint 3 backlog to latest versions
</commit_message>
<xml_diff>
--- a/documents/sprint backlog/sprint3/Sprint Backlog.xlsx
+++ b/documents/sprint backlog/sprint3/Sprint Backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
   <si>
     <t>User Stories</t>
   </si>
@@ -52,12 +52,6 @@
     <t>User Story</t>
   </si>
   <si>
-    <t>Task Number</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Michael:2</t>
   </si>
   <si>
@@ -67,16 +61,10 @@
     <t>Michael:1</t>
   </si>
   <si>
-    <t>Jacob:1</t>
+    <t>Jacob:2</t>
   </si>
   <si>
-    <t>Jerry 1</t>
-  </si>
-  <si>
-    <t>Jerry:2</t>
-  </si>
-  <si>
-    <t>Description</t>
+    <t>Jacob:1</t>
   </si>
   <si>
     <t>Gurpreet:1</t>
@@ -85,22 +73,22 @@
     <t>Gurpreet:2</t>
   </si>
   <si>
-    <t>Create query for top 10 languages of service</t>
+    <t>Task Number</t>
   </si>
   <si>
-    <t>Jacob:2</t>
-  </si>
-  <si>
-    <t>Jerry:3</t>
-  </si>
-  <si>
-    <t>Get total count for all languages from NeedsAccessRef</t>
+    <t>Name</t>
   </si>
   <si>
     <t>Jacob:3</t>
   </si>
   <si>
-    <t>Jacob:4</t>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Create query for top 10 languages of service</t>
+  </si>
+  <si>
+    <t>Get total count for all languages from NeedsAccessRef</t>
   </si>
   <si>
     <t>Create sample pre-set queries  as a drop down</t>
@@ -206,26 +194,26 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -250,6 +238,154 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Provisional and Actual</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burndown Chart'!$A$2</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="19050">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Burndown Chart'!$B$1:$I$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burndown Chart'!$B$2:$I$2</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burndown Chart'!$A$3</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="19050">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Burndown Chart'!$B$1:$I$1</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burndown Chart'!$B$3:$I$3</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="2139864880"/>
+        <c:axId val="658724892"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2139864880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="658724892"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="658724892"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2139864880"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
   <xdr:oneCellAnchor>
@@ -262,7 +398,7 @@
     <xdr:ext cx="6381750" cy="1162050"/>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Shape 5"/>
+        <xdr:cNvPr id="4" name="Shape 4"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -374,7 +510,7 @@
     <xdr:ext cx="6572250" cy="1066800"/>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Shape 4"/>
+        <xdr:cNvPr id="5" name="Shape 5"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -420,6 +556,31 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
@@ -471,34 +632,6 @@
     </xdr:sp>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -521,23 +654,23 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
+      <c r="B1" s="7" t="s">
+        <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>13</v>
+      <c r="C1" s="9" t="s">
+        <v>20</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>20</v>
+      <c r="F1" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -561,21 +694,21 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="10">
+      <c r="A2" s="8">
         <v>9.0</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="5">
         <v>26.0</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="7">
+      <c r="E2" s="5">
         <v>2.0</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -599,21 +732,21 @@
       <c r="Z2" s="3"/>
     </row>
     <row r="3">
-      <c r="A3" s="9">
+      <c r="A3" s="6">
         <v>10.0</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>27.0</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>3.0</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -637,21 +770,21 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>10.0</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>28.0</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>3.0</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -675,21 +808,21 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>10.0</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>29.0</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>3.0</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -713,23 +846,23 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="9">
-        <v>11.0</v>
+      <c r="A6" s="6">
+        <v>10.0</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>30.0</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>28.0</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>3.0</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -753,21 +886,21 @@
       <c r="Z6" s="3"/>
     </row>
     <row r="7">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>12.0</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>31.0</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>5.0</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -791,21 +924,21 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>12.0</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>32.0</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>5.0</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -28698,130 +28831,132 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>9.0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>26.0</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>2.0</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>27.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="B4" s="5">
+        <v>28.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="B5" s="6">
+        <v>29.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="B6" s="8">
+        <v>30.0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>28.0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="G6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="5">
-        <v>10.0</v>
+      <c r="H6" s="4" t="s">
+        <v>14</v>
       </c>
-      <c r="B3" s="7">
-        <v>27.0</v>
+      <c r="I6" s="4" t="s">
+        <v>14</v>
       </c>
-      <c r="D3" s="5">
-        <v>3.0</v>
+    </row>
+    <row r="7">
+      <c r="A7" s="4">
+        <v>12.0</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="B7" s="8">
+        <v>31.0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5">
-        <v>10.0</v>
-      </c>
-      <c r="B4" s="7">
-        <v>28.0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="5">
-        <v>10.0</v>
-      </c>
-      <c r="B5" s="9">
-        <v>29.0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="5">
-        <v>11.0</v>
-      </c>
-      <c r="B6" s="10">
-        <v>30.0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>28.0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5">
+    </row>
+    <row r="8">
+      <c r="A8" s="4">
         <v>12.0</v>
       </c>
-      <c r="B7" s="10">
-        <v>31.0</v>
+      <c r="B8" s="8">
+        <v>32.0</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D8" s="4">
         <v>5.0</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>19</v>
+      <c r="E8" s="4"/>
+      <c r="J8" s="4" t="s">
+        <v>15</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5">
-        <v>12.0</v>
-      </c>
-      <c r="B8" s="10">
-        <v>32.0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>5.0</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="J8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>27</v>
+      <c r="K8" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -28890,124 +29025,136 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>9.0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>26.0</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>2.0</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>27.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="5">
+    <row r="4">
+      <c r="A4" s="4">
         <v>10.0</v>
       </c>
-      <c r="B3" s="7">
-        <v>27.0</v>
+      <c r="B4" s="5">
+        <v>28.0</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D4" s="4">
         <v>3.0</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4">
         <v>10.0</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B5" s="6">
+        <v>29.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4">
+        <v>11.0</v>
+      </c>
+      <c r="B6" s="8">
+        <v>30.0</v>
+      </c>
+      <c r="C6" s="4">
         <v>28.0</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D6" s="4">
         <v>3.0</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>25</v>
+      <c r="G6" s="4" t="s">
+        <v>13</v>
       </c>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="5">
-        <v>10.0</v>
+      <c r="H6" s="4" t="s">
+        <v>14</v>
       </c>
-      <c r="B5" s="9">
-        <v>29.0</v>
+      <c r="I6" s="4" t="s">
+        <v>14</v>
       </c>
-      <c r="D5" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5">
-        <v>11.0</v>
-      </c>
-      <c r="B6" s="10">
-        <v>30.0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>28.0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>12.0</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="8">
         <v>31.0</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>5.0</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>24</v>
+      <c r="G7" s="4" t="s">
+        <v>15</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>27</v>
+      <c r="H7" s="4" t="s">
+        <v>15</v>
       </c>
+      <c r="I7" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>12.0</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <v>32.0</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>5.0</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="J8" s="5" t="s">
-        <v>28</v>
+      <c r="E8" s="4"/>
+      <c r="J8" s="4" t="s">
+        <v>15</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>17</v>
+      <c r="K8" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -29071,30 +29218,30 @@
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="8">
         <v>24.0</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="8">
         <v>22.0</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="8">
         <v>16.0</v>
       </c>
-      <c r="E2" s="10">
-        <v>10.0</v>
+      <c r="E2" s="8">
+        <v>13.0</v>
       </c>
-      <c r="F2" s="10">
-        <v>10.0</v>
+      <c r="F2" s="8">
+        <v>13.0</v>
       </c>
-      <c r="G2" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="H2" s="10">
+      <c r="G2" s="8">
         <v>5.0</v>
       </c>
-      <c r="I2" s="10">
+      <c r="H2" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="I2" s="8">
         <v>0.0</v>
       </c>
       <c r="J2" s="3"/>
@@ -29117,30 +29264,30 @@
     </row>
     <row r="3">
       <c r="A3" s="15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="8">
         <v>24.0</v>
       </c>
-      <c r="C3" s="10">
-        <v>21.0</v>
+      <c r="C3" s="8">
+        <v>24.0</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
+        <v>19.0</v>
+      </c>
+      <c r="E3" s="8">
         <v>16.0</v>
       </c>
-      <c r="E3" s="10">
+      <c r="F3" s="8">
         <v>13.0</v>
       </c>
-      <c r="F3" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="G3" s="10">
+      <c r="G3" s="8">
         <v>5.0</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="8">
         <v>5.0</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="8">
         <v>0.0</v>
       </c>
       <c r="J3" s="3"/>

</xml_diff>